<commit_message>
Create func to update columns
</commit_message>
<xml_diff>
--- a/src/datasrc/gbp_daily.xlsx
+++ b/src/datasrc/gbp_daily.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viclee/Developer/_gbfx/fx-research/src/datasrc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA5C039-B4AA-5A4F-9F7B-069961F00415}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157B0D5A-CEEB-5D40-B49C-53674E70825A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -897,7 +897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="338" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>

</xml_diff>